<commit_message>
Updated schedule and added memo
</commit_message>
<xml_diff>
--- a/Documents/Schedule.xlsx
+++ b/Documents/Schedule.xlsx
@@ -1055,13 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="B1:AY34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH9" sqref="AH9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -1656,7 +1653,7 @@
     </row>
     <row r="21" spans="2:29" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="15" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C21" s="14">
         <v>10</v>
@@ -1682,7 +1679,7 @@
     </row>
     <row r="22" spans="2:29" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="14">
         <v>10</v>
@@ -1708,13 +1705,13 @@
     </row>
     <row r="23" spans="2:29" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="15" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C23" s="14">
         <v>10</v>
       </c>
       <c r="D23" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" s="14">
         <v>0</v>
@@ -1726,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AA23"/>
       <c r="AB23"/>
@@ -1734,7 +1731,7 @@
     </row>
     <row r="24" spans="2:29" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="15" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C24" s="14">
         <v>10</v>
@@ -1749,10 +1746,10 @@
         <v>0</v>
       </c>
       <c r="G24" s="16">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AA24"/>
       <c r="AB24"/>
@@ -1760,9 +1757,9 @@
     </row>
     <row r="25" spans="2:29" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="17">
+        <v>29</v>
+      </c>
+      <c r="C25" s="14">
         <v>10</v>
       </c>
       <c r="D25" s="14">
@@ -1775,10 +1772,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="16">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA25"/>
       <c r="AB25"/>
@@ -1786,9 +1783,9 @@
     </row>
     <row r="26" spans="2:29" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="14">
+        <v>38</v>
+      </c>
+      <c r="C26" s="17">
         <v>10</v>
       </c>
       <c r="D26" s="14">
@@ -1812,7 +1809,7 @@
     </row>
     <row r="27" spans="2:29" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="14">
         <v>10</v>
@@ -1830,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AA27"/>
       <c r="AB27"/>
@@ -1838,13 +1835,13 @@
     </row>
     <row r="28" spans="2:29" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="14">
         <v>10</v>
       </c>
       <c r="D28" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="14">
         <v>0</v>
@@ -1856,7 +1853,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AA28"/>
       <c r="AB28"/>
@@ -2052,8 +2049,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="64" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>